<commit_message>
Arreglo de escritura y añadido de colores a las plantillas.
</commit_message>
<xml_diff>
--- a/src/main/resources/PlantillaSoluciones.xlsx
+++ b/src/main/resources/PlantillaSoluciones.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E92836C-326D-4FCC-AF44-FAE9E6CE3C1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solucion 1" sheetId="1" r:id="rId1"/>
@@ -68,7 +69,168 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="220">
+  <dxfs count="263">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9E644A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD99975"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -93,6 +255,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -100,6 +269,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFCCC0DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8E4BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA9694"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -107,6 +318,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF70FEC5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4EB87"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -114,6 +353,223 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD99975"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9E644A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCC0DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8E4BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA9694"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4EB87"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF70FEC5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -842,6 +1298,125 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4EB87"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF70FEC5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -849,6 +1424,146 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFCC9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA9694"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8E4BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCC0DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4EB87"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF70FEC5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -856,6 +1571,146 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA9694"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8E4BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCC0DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4EB87"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF70FEC5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
@@ -863,6 +1718,146 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA9694"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8E4BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCC0DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4EB87"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF70FEC5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
@@ -870,98 +1865,42 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4EB87"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF70FEC5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA9694"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8E4BC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -969,643 +1908,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFCCC0DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD8E4BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDA9694"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4EB87"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF70FEC5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDA9694"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD8E4BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCC0DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4EB87"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF70FEC5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCC0DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD8E4BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDA9694"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4EB87"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF70FEC5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCC0DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD8E4BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDA9694"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF70FEC5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4EB87"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCC0DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD8E4BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDA9694"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC9966"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1613,14 +1915,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9933"/>
+      <color rgb="FF9E644A"/>
+      <color rgb="FFD99975"/>
+      <color rgb="FF33CCCC"/>
+      <color rgb="FFFF66FF"/>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFFF5050"/>
       <color rgb="FF70FEC5"/>
       <color rgb="FFE4EB87"/>
       <color rgb="FF00B050"/>
-      <color rgb="FFCCC0DA"/>
-      <color rgb="FFD8E4BC"/>
-      <color rgb="FFDA9694"/>
-      <color rgb="FFCC9966"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1957,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="AE22:AP22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.5546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1982,73 +2286,106 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="219" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="64" priority="34" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="63" priority="33" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="62" priority="32" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="61" priority="31" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="199" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="35" priority="28" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="36" priority="29" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="37" priority="30" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="38" priority="24" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="39" priority="25" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="40" priority="23" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="41" priority="22" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="42" priority="21" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="20" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="19" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="18" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="17" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="16" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="15" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="14" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="13" operator="equal">
       <formula>"ABF"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="12" operator="containsText" text="acy">
+      <formula>NOT(ISERROR(SEARCH("acy",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="11" operator="containsText" text="ADU">
+      <formula>NOT(ISERROR(SEARCH("ADU",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="10" operator="containsText" text="ADF">
+      <formula>NOT(ISERROR(SEARCH("ADF",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="9" operator="containsText" text="AEA">
+      <formula>NOT(ISERROR(SEARCH("AEA",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="8" operator="containsText" text="ADL">
+      <formula>NOT(ISERROR(SEARCH("ADL",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="ADP">
+      <formula>NOT(ISERROR(SEARCH("ADP",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="ADQ">
+      <formula>NOT(ISERROR(SEARCH("ADQ",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="5" operator="containsText" text="ADR">
+      <formula>NOT(ISERROR(SEARCH("ADR",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="ADL">
+      <formula>NOT(ISERROR(SEARCH("ADL",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="3" operator="containsText" text="ADG">
+      <formula>NOT(ISERROR(SEARCH("ADG",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="ADK">
+      <formula>NOT(ISERROR(SEARCH("ADK",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2060,7 +2397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4790D87-1B48-4B8F-B2EF-DA67D43F5233}">
   <dimension ref="AE22:AP22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AQ27" sqref="AQ27"/>
     </sheetView>
   </sheetViews>
@@ -2085,72 +2422,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="86" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="85" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="84" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="83" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="74" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="73" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="72" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="71" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="70" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="69" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="68" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="66" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="65" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2188,72 +2525,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="194" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="262" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="261" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="260" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="259" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="176" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="250" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="249" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="248" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="247" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="246" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="245" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="244" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="243" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="242" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="241" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2296,72 +2633,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="172" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="240" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="239" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="238" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="237" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="154" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="228" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="227" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="226" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="225" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="224" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="223" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="222" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="221" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="220" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="219" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2399,72 +2736,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="153" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="218" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="217" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="216" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="215" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="149" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="206" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="205" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="204" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="203" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="202" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="201" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="200" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="199" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="198" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="197" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2502,72 +2839,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="128" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="196" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="195" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="194" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="193" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="110" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="184" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="183" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="182" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="181" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="180" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="179" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="178" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="177" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="176" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="175" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2605,72 +2942,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="109" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="174" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="173" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="172" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="171" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="105" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="162" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="161" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="160" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="159" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="158" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="157" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="156" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="155" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="154" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="153" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2708,72 +3045,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="87" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="152" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="151" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="150" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="149" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="83" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="140" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="139" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="138" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="137" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="136" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="135" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="134" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="133" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="132" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="131" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2811,72 +3148,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="65" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="130" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="129" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="128" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="127" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="61" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="118" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="117" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="116" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="115" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="114" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="113" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="112" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="111" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="110" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="109" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2914,72 +3251,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD21 A23:XFD1048576 A22:AE22 AQ22:XFD22">
-    <cfRule type="containsText" dxfId="43" priority="19" operator="containsText" text="AAW">
+    <cfRule type="containsText" dxfId="108" priority="19" operator="containsText" text="AAW">
       <formula>NOT(ISERROR(SEARCH("AAW",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="AAL">
+    <cfRule type="containsText" dxfId="107" priority="20" operator="containsText" text="AAL">
       <formula>NOT(ISERROR(SEARCH("AAL",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="21" operator="containsText" text="AAA">
+    <cfRule type="containsText" dxfId="106" priority="21" operator="containsText" text="AAA">
       <formula>NOT(ISERROR(SEARCH("AAA",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="22" operator="containsText" text="AAQ">
+    <cfRule type="containsText" dxfId="105" priority="22" operator="containsText" text="AAQ">
       <formula>NOT(ISERROR(SEARCH("AAQ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="1" operator="equal">
       <formula>"ABF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="2" operator="equal">
       <formula>"ABD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="3" operator="equal">
       <formula>"ABE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="4" operator="equal">
       <formula>"AAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="5" operator="equal">
       <formula>"AAV"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="6" operator="equal">
       <formula>"ABA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="7" operator="equal">
       <formula>"ABB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="8" operator="equal">
       <formula>"AAX"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="9" operator="containsText" text="AAM">
+    <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="AAM">
       <formula>NOT(ISERROR(SEARCH("AAM",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="AAT">
+    <cfRule type="containsText" dxfId="95" priority="10" operator="containsText" text="AAT">
       <formula>NOT(ISERROR(SEARCH("AAT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="AAF">
+    <cfRule type="containsText" dxfId="94" priority="11" operator="containsText" text="AAF">
       <formula>NOT(ISERROR(SEARCH("AAF",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="12" operator="containsText" text="AAO">
+    <cfRule type="containsText" dxfId="93" priority="12" operator="containsText" text="AAO">
       <formula>NOT(ISERROR(SEARCH("AAO",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="AAD">
+    <cfRule type="containsText" dxfId="92" priority="13" operator="containsText" text="AAD">
       <formula>NOT(ISERROR(SEARCH("AAD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="14" operator="containsText" text="AAR">
+    <cfRule type="containsText" dxfId="91" priority="14" operator="containsText" text="AAR">
       <formula>NOT(ISERROR(SEARCH("AAR",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="AAE">
+    <cfRule type="containsText" dxfId="90" priority="15" operator="containsText" text="AAE">
       <formula>NOT(ISERROR(SEARCH("AAE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="AAK">
+    <cfRule type="containsText" dxfId="89" priority="16" operator="containsText" text="AAK">
       <formula>NOT(ISERROR(SEARCH("AAK",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="AAJ">
+    <cfRule type="containsText" dxfId="88" priority="17" operator="containsText" text="AAJ">
       <formula>NOT(ISERROR(SEARCH("AAJ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="AAZ">
+    <cfRule type="containsText" dxfId="87" priority="18" operator="containsText" text="AAZ">
       <formula>NOT(ISERROR(SEARCH("AAZ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>